<commit_message>
working on scoring, answers are lagging
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\accidence-tester\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20681E6-E04D-4734-AE74-4C20459A7087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB8216-0A1F-4AF0-958B-D105A96FFFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{14C7D4AC-921B-4D81-B504-AEB9EE60565B}"/>
+    <workbookView xWindow="25080" yWindow="-9135" windowWidth="16440" windowHeight="28440" xr2:uid="{14C7D4AC-921B-4D81-B504-AEB9EE60565B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,42 +56,6 @@
     <t>Noun</t>
   </si>
   <si>
-    <t>singular nominative</t>
-  </si>
-  <si>
-    <t>singular accusative</t>
-  </si>
-  <si>
-    <t>singular vocative</t>
-  </si>
-  <si>
-    <t>singular genitive</t>
-  </si>
-  <si>
-    <t>singular dative</t>
-  </si>
-  <si>
-    <t>singular ablative</t>
-  </si>
-  <si>
-    <t>plural nominative</t>
-  </si>
-  <si>
-    <t>plural vocative</t>
-  </si>
-  <si>
-    <t>plural accusative</t>
-  </si>
-  <si>
-    <t>plural genitive</t>
-  </si>
-  <si>
-    <t>plural dative</t>
-  </si>
-  <si>
-    <t>plural ablative</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -168,6 +132,42 @@
   </si>
   <si>
     <t>ebus</t>
+  </si>
+  <si>
+    <t>singularnominative</t>
+  </si>
+  <si>
+    <t>singularvocative</t>
+  </si>
+  <si>
+    <t>singularaccusative</t>
+  </si>
+  <si>
+    <t>singulargenitive</t>
+  </si>
+  <si>
+    <t>singulardative</t>
+  </si>
+  <si>
+    <t>singularablative</t>
+  </si>
+  <si>
+    <t>pluralnominative</t>
+  </si>
+  <si>
+    <t>pluralvocative</t>
+  </si>
+  <si>
+    <t>pluralaccusative</t>
+  </si>
+  <si>
+    <t>pluralgenitive</t>
+  </si>
+  <si>
+    <t>pluraldative</t>
+  </si>
+  <si>
+    <t>pluralablative</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G9" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +547,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -589,10 +589,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -617,10 +617,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -631,10 +631,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -673,10 +673,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -687,10 +687,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -715,10 +715,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -771,10 +771,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -785,10 +785,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -799,10 +799,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -841,10 +841,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -883,10 +883,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -897,10 +897,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -925,10 +925,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -953,10 +953,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -995,10 +995,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1051,10 +1051,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1079,10 +1079,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1093,10 +1093,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -1219,10 +1219,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -1261,10 +1261,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -1345,10 +1345,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -1401,10 +1401,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
         <v>32</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -1555,10 +1555,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B77" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -1611,10 +1611,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
         <v>42</v>
-      </c>
-      <c r="B78" t="s">
-        <v>16</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>

</xml_diff>